<commit_message>
Create_roles_Excel (new class), changes in existing files (CreatePostExcel & CreatePostExcel_EditorRoles), admin.proprties, adminproperty.java, Excel_role creation (new excel file)
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/Excel_roleCreation.xlsx
+++ b/Aml_automation/src/Common/Excel_roleCreation.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17460" windowHeight="4920"/>
   </bookViews>
   <sheets>
     <sheet name="NewUser" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="B1:J14"/>
 </workbook>
 </file>
 
@@ -58,13 +59,13 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Description written here</t>
-  </si>
-  <si>
     <t>twitter user</t>
   </si>
   <si>
     <t>pankaj_testDirector8</t>
+  </si>
+  <si>
+    <t>Desc written here</t>
   </si>
 </sst>
 </file>
@@ -427,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -479,22 +480,22 @@
     </row>
     <row r="2" spans="1:10" ht="30">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>10</v>
@@ -503,7 +504,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>13</v>

</xml_diff>